<commit_message>
Fix trade closing functionality
</commit_message>
<xml_diff>
--- a/database/Account 3463.xlsx
+++ b/database/Account 3463.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,18 +526,30 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>OPEN</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+          <t>CLOSED</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>112</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1268</v>
+      </c>
       <c r="J2" s="2" t="n">
         <v>45725.84025475694</v>
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -583,6 +595,53 @@
       <c r="M3" t="inlineStr">
         <is>
           <t>TP</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>USDJPY</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>67</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>CLOSED</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>SL</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>-67</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1201</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>45727.40790072917</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>SL</t>
         </is>
       </c>
     </row>

</xml_diff>